<commit_message>
Added low-pass filter on outputs.
</commit_message>
<xml_diff>
--- a/LoPass.xlsx
+++ b/LoPass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\Reflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BC473A-AE94-4D8A-AC7B-24E315A718B6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8766F39A-69D0-4471-86BC-0DD8F3FE0834}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30105" windowHeight="15885" xr2:uid="{EE28F754-0172-4066-B0B6-EA68C3BCC341}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>AD8595 Filter Configuration</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>Output to ADC filter</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>fc</t>
   </si>
 </sst>
 </file>
@@ -60,7 +69,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -112,7 +121,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -429,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCBD4DB-60BC-4F57-9DEE-B32448B60B7C}">
-  <dimension ref="B4:D16"/>
+  <dimension ref="B4:D25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
@@ -503,6 +512,36 @@
         <v>15915.494309189537</v>
       </c>
     </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="3">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="3">
+        <f>1/(2*PI()*D22*D23)</f>
+        <v>33.862753849339441</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{B9F16794-D289-4C0C-9AD3-74E9D64D13D3}"/>

</xml_diff>